<commit_message>
added some more xpaths
</commit_message>
<xml_diff>
--- a/Xpath_sheet.xlsx
+++ b/Xpath_sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repo_Preeti\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{346DBF90-9963-4AA5-8D05-2AA98F7D588E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEA09ACA-601D-4905-8833-2AEC52B11A30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{DD4A8EFA-8F20-4557-8EF4-CC63D2F32AF9}"/>
   </bookViews>
@@ -25,10 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
-  <si>
-    <t>(For admin option)</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="55">
   <si>
     <t>ELEMENTS</t>
   </si>
@@ -42,9 +39,6 @@
     <t>//h6[@ class="oxd-text oxd-text--h6 oxd-topbar-header-breadcrumb-module"]</t>
   </si>
   <si>
-    <t>XPATHS---&gt;ORANGE HRM</t>
-  </si>
-  <si>
     <t>System users</t>
   </si>
   <si>
@@ -67,13 +61,142 @@
   </si>
   <si>
     <t>"?" Button</t>
+  </si>
+  <si>
+    <t>(FOR LOGIN PAGE)</t>
+  </si>
+  <si>
+    <t>orange hrm image</t>
+  </si>
+  <si>
+    <t>//img[@src="/web/images/ohrm_branding.png?v=1689053487449"]</t>
+  </si>
+  <si>
+    <t>login</t>
+  </si>
+  <si>
+    <t>//h5[@class="oxd-text oxd-text--h5 orangehrm-login-title"]</t>
+  </si>
+  <si>
+    <t>//label[text()="Username"]</t>
+  </si>
+  <si>
+    <t>(ORANGE HRM,admin section)</t>
+  </si>
+  <si>
+    <t>textbox of username</t>
+  </si>
+  <si>
+    <t>//input[@class="oxd-input oxd-input--active" and @name="username"]</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>//label[text()="Password"]</t>
+  </si>
+  <si>
+    <t>textbox of password</t>
+  </si>
+  <si>
+    <t>//input[@class="oxd-input oxd-input--active" and @name="password"]</t>
+  </si>
+  <si>
+    <t>login button</t>
+  </si>
+  <si>
+    <t>//button[@class="oxd-button oxd-button--medium oxd-button--main orangehrm-login-button"]</t>
+  </si>
+  <si>
+    <t>forgot your password</t>
+  </si>
+  <si>
+    <t>//p[@class="oxd-text oxd-text--p orangehrm-login-forgot-header"]</t>
+  </si>
+  <si>
+    <t>OrangeHrm.Inc</t>
+  </si>
+  <si>
+    <t>//a[@href="http://www.orangehrm.com"]</t>
+  </si>
+  <si>
+    <t>login whole block</t>
+  </si>
+  <si>
+    <t>//div[@class="orangehrm-login-branding"]</t>
+  </si>
+  <si>
+    <t>(DASHBOARD)</t>
+  </si>
+  <si>
+    <t>Dashboard (Heading)</t>
+  </si>
+  <si>
+    <t>//h6[@class="oxd-text oxd-text--h6 oxd-topbar-header-breadcrumb-module"]</t>
+  </si>
+  <si>
+    <t>some button</t>
+  </si>
+  <si>
+    <t>//button[@class="oxd-icon-button oxd-icon-button--success orangehrm-report-icon"]</t>
+  </si>
+  <si>
+    <t>//p[@class="oxd-userdropdown-name"]</t>
+  </si>
+  <si>
+    <t>(13) Leave Requests to Approve</t>
+  </si>
+  <si>
+    <t>//div[@class="orangehrm-dashboard-widget-name" and i[@class="oxd-icon bi-lightning-charge-fill orangehrm-dashboard-widget-icon"]]</t>
+  </si>
+  <si>
+    <t>XPATHS FOR ORANGE HRM APPLICATION</t>
+  </si>
+  <si>
+    <t>symbol with Quick Launch</t>
+  </si>
+  <si>
+    <t>//*[local-name()='svg' and @class="oxd-icon oxd-menu-icon"]</t>
+  </si>
+  <si>
+    <t>Search symbol</t>
+  </si>
+  <si>
+    <t>//div[@class="orangehrm-attendance-card-summary-total"]</t>
+  </si>
+  <si>
+    <t>timer symbol with 64hr 32m</t>
+  </si>
+  <si>
+    <t>symbol beside employee on leave today</t>
+  </si>
+  <si>
+    <t>//*[local-name()='svg' and @class="oxd-icon orangehrm-dashboard-widget-icon"]</t>
+  </si>
+  <si>
+    <t>pie chart</t>
+  </si>
+  <si>
+    <t>//canvas[@id="ULgGz_5L"]</t>
+  </si>
+  <si>
+    <t>happy birthday image</t>
+  </si>
+  <si>
+    <t>//img[@class="orangehrm-buzz-widget-picture"]</t>
+  </si>
+  <si>
+    <t>timer symbol</t>
+  </si>
+  <si>
+    <t>//button[@class="oxd-icon-button oxd-icon-button--solid-main orangehrm-attendance-card-action"]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -91,7 +214,23 @@
     </font>
     <font>
       <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -118,12 +257,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -439,84 +585,255 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89A5B0D2-6FEE-4001-A353-B7DCE7CF0437}">
-  <dimension ref="A1:J12"/>
+  <dimension ref="A1:J40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.88671875" customWidth="1"/>
-    <col min="2" max="2" width="73.5546875" customWidth="1"/>
-    <col min="3" max="3" width="36.5546875" customWidth="1"/>
+    <col min="1" max="1" width="33.6640625" customWidth="1"/>
+    <col min="2" max="2" width="117.33203125" customWidth="1"/>
+    <col min="3" max="3" width="17.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="C1" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="B1" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" s="1"/>
       <c r="J1" s="1"/>
     </row>
     <row r="3" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>0</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>1</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" t="s">
         <v>3</v>
-      </c>
-      <c r="B7" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
         <v>13</v>
       </c>
-      <c r="B12" t="s">
-        <v>12</v>
+      <c r="B17" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>23</v>
+      </c>
+      <c r="B22" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>25</v>
+      </c>
+      <c r="B23" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>27</v>
+      </c>
+      <c r="B24" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B25" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>31</v>
+      </c>
+      <c r="B26" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A29" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>34</v>
+      </c>
+      <c r="B31" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>36</v>
+      </c>
+      <c r="B32" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>39</v>
+      </c>
+      <c r="B33" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>42</v>
+      </c>
+      <c r="B34" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>44</v>
+      </c>
+      <c r="B35" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B36" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>47</v>
+      </c>
+      <c r="B37" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>49</v>
+      </c>
+      <c r="B38" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>51</v>
+      </c>
+      <c r="B39" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>53</v>
+      </c>
+      <c r="B40" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated xpath excel file
</commit_message>
<xml_diff>
--- a/Xpath_sheet.xlsx
+++ b/Xpath_sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repo_Preeti\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DC03D18-6EB0-4693-BF69-398EE7C4FEC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{555494B9-FC7D-4F6F-80C6-C6AC9A07524D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{DD4A8EFA-8F20-4557-8EF4-CC63D2F32AF9}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="173">
   <si>
     <t>ELEMENTS</t>
   </si>
@@ -383,6 +383,207 @@
   </si>
   <si>
     <t>Switch on and off button</t>
+  </si>
+  <si>
+    <t>*Required</t>
+  </si>
+  <si>
+    <t>//p[@class="oxd-text oxd-text--p orangehrm-form-hint"]</t>
+  </si>
+  <si>
+    <t>(leave list)</t>
+  </si>
+  <si>
+    <t>(User Management)</t>
+  </si>
+  <si>
+    <t>(Corporate Branding)</t>
+  </si>
+  <si>
+    <t>Corporate Branding</t>
+  </si>
+  <si>
+    <t>image at profile picture</t>
+  </si>
+  <si>
+    <t>//img[@class="oxd-userdropdown-img"]</t>
+  </si>
+  <si>
+    <t>//div[@class="oxd-color-input oxd-color-input--active" and div[@class="oxd-color-input-preview" and @style="background-color: rgb(255, 123, 29); opacity: 1; cursor: pointer;"]]</t>
+  </si>
+  <si>
+    <t>circle with colour filled</t>
+  </si>
+  <si>
+    <t>Switch on off button</t>
+  </si>
+  <si>
+    <t>Primary color* with circle infront of it</t>
+  </si>
+  <si>
+    <t>//div[@class="orangehrm-color-input-wrapper" and label[@class="oxd-label oxd-input-field-required" and text()="Primary Color"]]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Primary color* </t>
+  </si>
+  <si>
+    <t>//label[text()="Primary Color"]</t>
+  </si>
+  <si>
+    <t>Publish button</t>
+  </si>
+  <si>
+    <t>combination of reset, default and publish buttons</t>
+  </si>
+  <si>
+    <t>//div[@class="orangehrm-actions-group"]</t>
+  </si>
+  <si>
+    <t>social media images with switch on off button</t>
+  </si>
+  <si>
+    <t>//div[@class="orangehrm-sm-field"]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">some text </t>
+  </si>
+  <si>
+    <t>//p[text()="Accepts jpg, .png, .gif, .svg up to 1MB. Recommended dimensions: 50px X 50px"]</t>
+  </si>
+  <si>
+    <t>//i[@class="oxd-icon bi-x --clear"]</t>
+  </si>
+  <si>
+    <t>Pending Approval with cross sign</t>
+  </si>
+  <si>
+    <t>//span[@class="oxd-chip oxd-chip--default oxd-multiselect-chips-selected"]      ( or )        //span[text()="Pending Approval "]</t>
+  </si>
+  <si>
+    <t>//h6[text()="Corporate Branding"]        (or)        //h6[@class="oxd-text oxd-text--h6 orangehrm-main-title"]</t>
+  </si>
+  <si>
+    <t>three vertical dots</t>
+  </si>
+  <si>
+    <t>//i[@class="oxd-icon bi-three-dots-vertical"]</t>
+  </si>
+  <si>
+    <t>whole three vertical dot button</t>
+  </si>
+  <si>
+    <t>//button[@class="oxd-icon-button" and @type="button" and i[@class="oxd-icon bi-three-dots-vertical"] ]</t>
+  </si>
+  <si>
+    <t>//div[@class="oxd-table-header-cell oxd-padding-cell oxd-table-th" and @role="columnheader" and div[@class="oxd-checkbox-wrapper"]]</t>
+  </si>
+  <si>
+    <t>check box beside date</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>//div[@class="oxd-table-header-cell oxd-padding-cell oxd-table-th" and text()="Date" ]</t>
+  </si>
+  <si>
+    <t>//div[ text()="2023-08-04 to 2023-08-10" ]</t>
+  </si>
+  <si>
+    <t>2023-08-04 to 2023-08-10</t>
+  </si>
+  <si>
+    <t>divider line</t>
+  </si>
+  <si>
+    <t>//div[@class="orangehrm-bottom-container"]</t>
+  </si>
+  <si>
+    <t>(Reports)</t>
+  </si>
+  <si>
+    <t>four side arrows</t>
+  </si>
+  <si>
+    <t>//i[@class="oxd-icon bi-arrows-fullscreen oxd-icon-button__icon --toggable-icon"]</t>
+  </si>
+  <si>
+    <t>//i[@class="oxd-icon bi-chevron-left oxd-icon-button__icon --toggable-icon"]</t>
+  </si>
+  <si>
+    <t>&lt;</t>
+  </si>
+  <si>
+    <t>&gt;</t>
+  </si>
+  <si>
+    <t>//i[@class="oxd-icon bi-chevron-right oxd-icon-button__icon --toggable-icon"]</t>
+  </si>
+  <si>
+    <t>combine of above three</t>
+  </si>
+  <si>
+    <t>//div[@class="oxd-report-table-header--toggable"]</t>
+  </si>
+  <si>
+    <t>Leave period text box</t>
+  </si>
+  <si>
+    <t>//div[@class="oxd-select-text-input"]</t>
+  </si>
+  <si>
+    <t>//div[@class="oxd-select-text oxd-select-text--active"]</t>
+  </si>
+  <si>
+    <t>text inside text box</t>
+  </si>
+  <si>
+    <t>//i[@class="oxd-icon bi-caret-down-fill oxd-select-text--arrow"]</t>
+  </si>
+  <si>
+    <t>side scroller</t>
+  </si>
+  <si>
+    <t>//revogr-scroll-virtual [@class="horizontal"]</t>
+  </si>
+  <si>
+    <t>(MY INFO)</t>
+  </si>
+  <si>
+    <t>//h6[@class="oxd-text oxd-text--h6 --strong"]</t>
+  </si>
+  <si>
+    <t>PaulTom Smasher</t>
+  </si>
+  <si>
+    <t>Profile picture</t>
+  </si>
+  <si>
+    <t>//img[@class="employee-image"]</t>
+  </si>
+  <si>
+    <t>Emplyoee full name</t>
+  </si>
+  <si>
+    <t>//label[@class="oxd-label oxd-input-field-required"]</t>
+  </si>
+  <si>
+    <t>text box to enter first name</t>
+  </si>
+  <si>
+    <t>//input[@class="oxd-input oxd-input--active orangehrm-firstname"]</t>
+  </si>
+  <si>
+    <t>Personal details</t>
+  </si>
+  <si>
+    <t>//a[@class="orangehrm-tabs-item --active"]</t>
+  </si>
+  <si>
+    <t>radio button</t>
+  </si>
+  <si>
+    <t>//input[@value="1"  ]</t>
   </si>
 </sst>
 </file>
@@ -458,7 +659,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -473,6 +674,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -488,6 +690,71 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>30480</xdr:colOff>
+      <xdr:row>87</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>175260</xdr:colOff>
+      <xdr:row>88</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Multiplication Sign 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D6FD71AE-2C7A-8699-7FF8-6248EFE6F621}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="30480" y="15933420"/>
+          <a:ext cx="144780" cy="182880"/>
+        </a:xfrm>
+        <a:prstGeom prst="mathMultiply">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-IN" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -787,16 +1054,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89A5B0D2-6FEE-4001-A353-B7DCE7CF0437}">
-  <dimension ref="A1:J69"/>
+  <dimension ref="A1:J114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="A69" sqref="A69"/>
+    <sheetView tabSelected="1" topLeftCell="A95" workbookViewId="0">
+      <selection activeCell="A115" sqref="A115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="40" customWidth="1"/>
-    <col min="2" max="2" width="117.33203125" customWidth="1"/>
+    <col min="1" max="1" width="43.109375" customWidth="1"/>
+    <col min="2" max="2" width="145" customWidth="1"/>
     <col min="3" max="3" width="17.88671875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -820,33 +1087,30 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>2</v>
-      </c>
-      <c r="B7" t="s">
-        <v>3</v>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" s="7" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B8" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B10" t="s">
         <v>6</v>
@@ -854,405 +1118,698 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>8</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B12" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+    <row r="13" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
         <v>69</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B13" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
         <v>61</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B14" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+    <row r="15" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
         <v>63</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B15" t="s">
         <v>64</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>65</v>
-      </c>
-      <c r="B15" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="B16" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B17" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B18" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B19" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B20" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B21" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B22" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B23" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B24" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B25" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B26" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B27" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B28" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B29" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
+        <v>98</v>
+      </c>
+      <c r="B30" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
         <v>101</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B31" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A33" s="2" t="s">
-        <v>11</v>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" s="7" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>12</v>
+        <v>111</v>
       </c>
       <c r="B35" t="s">
-        <v>13</v>
+        <v>131</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>14</v>
+        <v>112</v>
       </c>
       <c r="B36" t="s">
-        <v>15</v>
+        <v>113</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>7</v>
+        <v>115</v>
       </c>
       <c r="B37" t="s">
-        <v>16</v>
+        <v>114</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>18</v>
+        <v>116</v>
       </c>
       <c r="B38" t="s">
-        <v>19</v>
+        <v>104</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>20</v>
+        <v>117</v>
       </c>
       <c r="B39" t="s">
-        <v>21</v>
+        <v>118</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>22</v>
+        <v>119</v>
       </c>
       <c r="B40" t="s">
-        <v>23</v>
+        <v>120</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>24</v>
+        <v>121</v>
       </c>
       <c r="B41" t="s">
-        <v>25</v>
+        <v>84</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>26</v>
+        <v>122</v>
       </c>
       <c r="B42" t="s">
-        <v>27</v>
+        <v>123</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A43" s="4" t="s">
-        <v>28</v>
+      <c r="A43" t="s">
+        <v>124</v>
       </c>
       <c r="B43" t="s">
-        <v>29</v>
+        <v>125</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>30</v>
+        <v>126</v>
       </c>
       <c r="B44" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A47" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A49" t="s">
-        <v>33</v>
-      </c>
-      <c r="B49" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A50" t="s">
-        <v>35</v>
-      </c>
-      <c r="B50" t="s">
-        <v>36</v>
+        <v>127</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A49" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>38</v>
+        <v>12</v>
       </c>
       <c r="B51" t="s">
-        <v>37</v>
+        <v>13</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>41</v>
+        <v>14</v>
       </c>
       <c r="B52" t="s">
-        <v>39</v>
+        <v>15</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>43</v>
+        <v>7</v>
       </c>
       <c r="B53" t="s">
-        <v>42</v>
+        <v>16</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A54" s="6" t="s">
-        <v>45</v>
+      <c r="A54" t="s">
+        <v>18</v>
       </c>
       <c r="B54" t="s">
-        <v>44</v>
+        <v>19</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>46</v>
+        <v>20</v>
       </c>
       <c r="B55" t="s">
-        <v>47</v>
+        <v>21</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>48</v>
+        <v>22</v>
       </c>
       <c r="B56" t="s">
-        <v>49</v>
+        <v>23</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>50</v>
+        <v>24</v>
       </c>
       <c r="B57" t="s">
-        <v>51</v>
+        <v>25</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>52</v>
+        <v>26</v>
       </c>
       <c r="B58" t="s">
-        <v>53</v>
+        <v>27</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A59" t="s">
-        <v>54</v>
+      <c r="A59" s="4" t="s">
+        <v>28</v>
       </c>
       <c r="B59" t="s">
-        <v>55</v>
+        <v>29</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>56</v>
+        <v>30</v>
       </c>
       <c r="B60" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A61" t="s">
-        <v>58</v>
-      </c>
-      <c r="B61" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A62" t="s">
-        <v>60</v>
-      </c>
-      <c r="B62" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A63" t="s">
-        <v>67</v>
-      </c>
-      <c r="B63" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A64" t="s">
-        <v>70</v>
-      </c>
-      <c r="B64" t="s">
-        <v>71</v>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A63" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>33</v>
+      </c>
+      <c r="B65" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A66" s="7" t="s">
-        <v>102</v>
+      <c r="A66" t="s">
+        <v>35</v>
+      </c>
+      <c r="B66" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>38</v>
+      </c>
+      <c r="B67" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>103</v>
+        <v>41</v>
       </c>
       <c r="B68" t="s">
-        <v>5</v>
+        <v>39</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
+        <v>43</v>
+      </c>
+      <c r="B69" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A70" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B70" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
+        <v>46</v>
+      </c>
+      <c r="B71" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
+        <v>48</v>
+      </c>
+      <c r="B72" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
+        <v>50</v>
+      </c>
+      <c r="B73" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
+        <v>52</v>
+      </c>
+      <c r="B74" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
+        <v>54</v>
+      </c>
+      <c r="B75" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
+        <v>56</v>
+      </c>
+      <c r="B76" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A77" t="s">
+        <v>58</v>
+      </c>
+      <c r="B77" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
+        <v>60</v>
+      </c>
+      <c r="B78" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A79" t="s">
+        <v>67</v>
+      </c>
+      <c r="B79" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
+        <v>70</v>
+      </c>
+      <c r="B80" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A82" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A83" s="7"/>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A84" s="7" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A85" t="s">
+        <v>103</v>
+      </c>
+      <c r="B85" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A86" t="s">
         <v>105</v>
       </c>
-      <c r="B69" t="s">
+      <c r="B86" t="s">
         <v>104</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A87" t="s">
+        <v>106</v>
+      </c>
+      <c r="B87" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B88" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A89" t="s">
+        <v>129</v>
+      </c>
+      <c r="B89" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A90" t="s">
+        <v>132</v>
+      </c>
+      <c r="B90" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A91" t="s">
+        <v>134</v>
+      </c>
+      <c r="B91" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A92" t="s">
+        <v>137</v>
+      </c>
+      <c r="B92" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A93" t="s">
+        <v>138</v>
+      </c>
+      <c r="B93" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A94" t="s">
+        <v>141</v>
+      </c>
+      <c r="B94" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A95" t="s">
+        <v>142</v>
+      </c>
+      <c r="B95" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A97" s="7" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A98" t="s">
+        <v>145</v>
+      </c>
+      <c r="B98" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A99" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="B99" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A100" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="B100" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A101" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="B101" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A102" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="B102" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A103" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="B103" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A104" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="B104" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A105" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="B105" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A107" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A109" t="s">
+        <v>162</v>
+      </c>
+      <c r="B109" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A110" t="s">
+        <v>163</v>
+      </c>
+      <c r="B110" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A111" t="s">
+        <v>165</v>
+      </c>
+      <c r="B111" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A112" t="s">
+        <v>167</v>
+      </c>
+      <c r="B112" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A113" t="s">
+        <v>169</v>
+      </c>
+      <c r="B113" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A114" t="s">
+        <v>171</v>
+      </c>
+      <c r="B114" t="s">
+        <v>172</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>